<commit_message>
fill ipa like matrix
</commit_message>
<xml_diff>
--- a/ipa_like_matrix.xlsx
+++ b/ipa_like_matrix.xlsx
@@ -705,10 +705,10 @@
   <dimension ref="A1:BV74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="P1" sqref="P1"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AN11" sqref="AN11"/>
+      <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
@@ -720,24 +720,25 @@
     <col min="7" max="11" width="3.125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="2.875" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="3.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="2.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="3.125" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="3.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="2.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.125" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="3.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="28" width="2.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="3.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="2.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="3.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="3.125" style="2" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="3.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="2.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="3.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="2.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="3.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="39" width="3.125" style="2" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="3.625" style="2" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="5.125" style="2" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="3.5" style="2" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="3.125" style="2" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="2.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="2.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="3.125" style="2" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="3.625" style="2" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="2.875" style="2" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="4.625" style="2" bestFit="1" customWidth="1"/>
@@ -1303,13 +1304,17 @@
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
+      <c r="Z5" s="1">
+        <v>1</v>
+      </c>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
+      <c r="AF5" s="1">
+        <v>1</v>
+      </c>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
@@ -1323,7 +1328,9 @@
       <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
       <c r="AS5" s="1"/>
-      <c r="AT5" s="1"/>
+      <c r="AT5" s="1">
+        <v>1</v>
+      </c>
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
       <c r="AW5" s="1"/>
@@ -1563,13 +1570,17 @@
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
+      <c r="Z8" s="1">
+        <v>1</v>
+      </c>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
-      <c r="AF8" s="1"/>
+      <c r="AF8" s="1">
+        <v>1</v>
+      </c>
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
@@ -1583,7 +1594,9 @@
       <c r="AQ8" s="1"/>
       <c r="AR8" s="1"/>
       <c r="AS8" s="1"/>
-      <c r="AT8" s="1"/>
+      <c r="AT8" s="1">
+        <v>1</v>
+      </c>
       <c r="AU8" s="1"/>
       <c r="AV8" s="1"/>
       <c r="AW8" s="1"/>
@@ -1902,10 +1915,18 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
+      <c r="Q12" s="1">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1">
+        <v>1</v>
+      </c>
+      <c r="S12" s="1">
+        <v>1</v>
+      </c>
+      <c r="T12" s="1">
+        <v>1</v>
+      </c>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
@@ -1988,7 +2009,9 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
+      <c r="W13" s="1">
+        <v>1</v>
+      </c>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
@@ -2074,8 +2097,12 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
+      <c r="AC14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="1">
+        <v>1</v>
+      </c>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
@@ -2303,9 +2330,15 @@
       <c r="Q17" s="1">
         <v>1</v>
       </c>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
+      <c r="R17" s="1">
+        <v>1</v>
+      </c>
+      <c r="S17" s="1">
+        <v>1</v>
+      </c>
+      <c r="T17" s="1">
+        <v>1</v>
+      </c>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
@@ -2313,7 +2346,9 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
+      <c r="AB17" s="1">
+        <v>1</v>
+      </c>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
@@ -2384,8 +2419,12 @@
       <c r="R18" s="1">
         <v>1</v>
       </c>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
+      <c r="S18" s="1">
+        <v>1</v>
+      </c>
+      <c r="T18" s="1">
+        <v>1</v>
+      </c>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
@@ -2465,7 +2504,9 @@
       <c r="S19" s="1">
         <v>1</v>
       </c>
-      <c r="T19" s="1"/>
+      <c r="T19" s="1">
+        <v>1</v>
+      </c>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
@@ -2637,11 +2678,17 @@
       <c r="AC21" s="1"/>
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
-      <c r="AF21" s="1"/>
-      <c r="AG21" s="1"/>
+      <c r="AF21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="1">
+        <v>1</v>
+      </c>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
-      <c r="AJ21" s="1"/>
+      <c r="AJ21" s="1">
+        <v>1</v>
+      </c>
       <c r="AK21" s="1"/>
       <c r="AL21" s="1"/>
       <c r="AM21" s="1"/>
@@ -2652,7 +2699,9 @@
       <c r="AR21" s="1"/>
       <c r="AS21" s="1"/>
       <c r="AT21" s="1"/>
-      <c r="AU21" s="1"/>
+      <c r="AU21" s="1">
+        <v>1</v>
+      </c>
       <c r="AV21" s="1"/>
       <c r="AW21" s="1"/>
       <c r="AX21" s="1"/>
@@ -2722,11 +2771,15 @@
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
-      <c r="AK22" s="1"/>
+      <c r="AK22" s="1">
+        <v>1</v>
+      </c>
       <c r="AL22" s="1"/>
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
-      <c r="AO22" s="1"/>
+      <c r="AO22" s="1">
+        <v>1</v>
+      </c>
       <c r="AP22" s="1"/>
       <c r="AQ22" s="1"/>
       <c r="AR22" s="1"/>
@@ -2870,7 +2923,9 @@
       <c r="X24" s="1">
         <v>1</v>
       </c>
-      <c r="Y24" s="1"/>
+      <c r="Y24" s="1">
+        <v>1</v>
+      </c>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
@@ -2884,8 +2939,12 @@
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
       <c r="AL24" s="1"/>
-      <c r="AM24" s="1"/>
-      <c r="AN24" s="1"/>
+      <c r="AM24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN24" s="1">
+        <v>1</v>
+      </c>
       <c r="AO24" s="1"/>
       <c r="AP24" s="1"/>
       <c r="AQ24" s="1"/>
@@ -2964,8 +3023,12 @@
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
       <c r="AL25" s="1"/>
-      <c r="AM25" s="1"/>
-      <c r="AN25" s="1"/>
+      <c r="AM25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN25" s="1">
+        <v>1</v>
+      </c>
       <c r="AO25" s="1"/>
       <c r="AP25" s="1"/>
       <c r="AQ25" s="1"/>
@@ -3037,7 +3100,9 @@
       <c r="AC26" s="1"/>
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
-      <c r="AF26" s="1"/>
+      <c r="AF26" s="1">
+        <v>1</v>
+      </c>
       <c r="AG26" s="1"/>
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
@@ -3051,7 +3116,9 @@
       <c r="AQ26" s="1"/>
       <c r="AR26" s="1"/>
       <c r="AS26" s="1"/>
-      <c r="AT26" s="1"/>
+      <c r="AT26" s="1">
+        <v>1</v>
+      </c>
       <c r="AU26" s="1"/>
       <c r="AV26" s="1"/>
       <c r="AW26" s="1"/>
@@ -3275,7 +3342,9 @@
       <c r="AC29" s="1">
         <v>1</v>
       </c>
-      <c r="AD29" s="1"/>
+      <c r="AD29" s="1">
+        <v>1</v>
+      </c>
       <c r="AE29" s="1"/>
       <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
@@ -3288,7 +3357,9 @@
       <c r="AN29" s="1"/>
       <c r="AO29" s="1"/>
       <c r="AP29" s="1"/>
-      <c r="AQ29" s="1"/>
+      <c r="AQ29" s="1">
+        <v>1</v>
+      </c>
       <c r="AR29" s="1"/>
       <c r="AS29" s="1"/>
       <c r="AT29" s="1"/>
@@ -3368,7 +3439,9 @@
       <c r="AN30" s="1"/>
       <c r="AO30" s="1"/>
       <c r="AP30" s="1"/>
-      <c r="AQ30" s="1"/>
+      <c r="AQ30" s="1">
+        <v>1</v>
+      </c>
       <c r="AR30" s="1"/>
       <c r="AS30" s="1"/>
       <c r="AT30" s="1"/>
@@ -3531,7 +3604,9 @@
       <c r="AQ32" s="1"/>
       <c r="AR32" s="1"/>
       <c r="AS32" s="1"/>
-      <c r="AT32" s="1"/>
+      <c r="AT32" s="1">
+        <v>1</v>
+      </c>
       <c r="AU32" s="1"/>
       <c r="AV32" s="1"/>
       <c r="AW32" s="1"/>
@@ -3601,7 +3676,9 @@
       </c>
       <c r="AH33" s="1"/>
       <c r="AI33" s="1"/>
-      <c r="AJ33" s="1"/>
+      <c r="AJ33" s="1">
+        <v>1</v>
+      </c>
       <c r="AK33" s="1"/>
       <c r="AL33" s="1"/>
       <c r="AM33" s="1"/>
@@ -3612,7 +3689,9 @@
       <c r="AR33" s="1"/>
       <c r="AS33" s="1"/>
       <c r="AT33" s="1"/>
-      <c r="AU33" s="1"/>
+      <c r="AU33" s="1">
+        <v>1</v>
+      </c>
       <c r="AV33" s="1"/>
       <c r="AW33" s="1"/>
       <c r="AX33" s="1"/>
@@ -3680,7 +3759,9 @@
       <c r="AH34" s="1">
         <v>1</v>
       </c>
-      <c r="AI34" s="1"/>
+      <c r="AI34" s="1">
+        <v>1</v>
+      </c>
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
       <c r="AL34" s="1"/>
@@ -3926,7 +4007,9 @@
       <c r="AL37" s="1"/>
       <c r="AM37" s="1"/>
       <c r="AN37" s="1"/>
-      <c r="AO37" s="1"/>
+      <c r="AO37" s="1">
+        <v>1</v>
+      </c>
       <c r="AP37" s="1"/>
       <c r="AQ37" s="1"/>
       <c r="AR37" s="1"/>

</xml_diff>